<commit_message>
fix sample import report
</commit_message>
<xml_diff>
--- a/public/sample/sample_import_report.xlsx
+++ b/public/sample/sample_import_report.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/didi/project/taxsam-sia-2022/public/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1D70A1-3746-4448-B9A2-35CA374326C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F9C89B-1CAB-A34D-9F45-3DC5264D42DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="500" windowWidth="21680" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LAPORAN 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Laporan Dasar" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>

</xml_diff>